<commit_message>
rebuild compas tests utilizing propublica dataset
</commit_message>
<xml_diff>
--- a/compas-tests/atributos e descrições.xlsx
+++ b/compas-tests/atributos e descrições.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Downloads\Temporario\fairness-testing\compas-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AB0519-C8EF-49B6-814B-332D93F7B3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B897DCB3-3BCA-4809-8B95-F96E4B70AB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -279,9 +279,6 @@
     <t>categoria do nível de decisão de reincidência (low, medium, high)</t>
   </si>
   <si>
-    <t>categoria do nível de decisão de reincidência (lowScore, highScore)</t>
-  </si>
-  <si>
     <t>data de entrada da prisão</t>
   </si>
   <si>
@@ -340,6 +337,9 @@
   </si>
   <si>
     <t>coluna repetida</t>
+  </si>
+  <si>
+    <t>categoria do nível de previsão de reincidência (lowScore, highScore)</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -752,7 +754,7 @@
       <c r="C3" s="2"/>
       <c r="E3" s="10"/>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -764,7 +766,7 @@
       </c>
       <c r="E4" s="11"/>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -776,7 +778,7 @@
       </c>
       <c r="E5" s="12"/>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -888,7 +890,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -920,7 +922,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -928,7 +930,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -944,7 +946,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -960,7 +962,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -968,7 +970,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -976,7 +978,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -984,7 +986,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -992,7 +994,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -1000,7 +1002,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -1008,7 +1010,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -1016,7 +1018,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -1024,7 +1026,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -1032,7 +1034,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
@@ -1040,7 +1042,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -1048,7 +1050,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -1056,7 +1058,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
@@ -1178,7 +1180,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>